<commit_message>
mouseInteraction implementation stage #2
</commit_message>
<xml_diff>
--- a/documentation/Mouse interaction.xlsx
+++ b/documentation/Mouse interaction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Joshl\Documents\GitHub\traffic-simulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06140123-924B-4C93-94A5-97A4FF054390}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAF59F9-B4BE-4EEF-B18C-FD88E5B9F0C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF97C960-519B-467F-9B64-B777376BEA9A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>MouseInteraction</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>Move canvas origin using mouse position</t>
+  </si>
+  <si>
+    <t>Mouse wheel moved</t>
+  </si>
+  <si>
+    <t>Zoom canvas</t>
+  </si>
+  <si>
+    <t>Move vertex</t>
+  </si>
+  <si>
+    <t>Created isolated node</t>
+  </si>
+  <si>
+    <t>shift-click vertex</t>
   </si>
 </sst>
 </file>
@@ -460,7 +475,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,6 +556,12 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -555,6 +576,12 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -569,6 +596,12 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -583,6 +616,12 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -605,6 +644,12 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -624,5 +669,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>